<commit_message>
added more details to schedule
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6351DC9-38F1-440A-81CD-6DD1FD3486CD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F2BDA4-B14A-49BE-A59C-75BABA1F8251}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1155" yWindow="-180" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,11 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <t>Planned</t>
-    <phoneticPr fontId="1"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Completed</t>
     <phoneticPr fontId="1"/>
@@ -54,34 +50,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Deep Q Agent for Gym MountainCarContinous</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Deep Q Agent for Gym Acrobat</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Deep Q Agent for Gym Cartpole</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Deep Q Agent for Gym Pendulum</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>DDPG Agent for Gym MountainCarContinous</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>DDPG Agent for Gym Cartpole</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>DDPG Agent for Gym Acrobat</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>DDPG Agent for Gym Pendulum</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -107,6 +79,52 @@
   </si>
   <si>
     <t>CarRacing-V0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://towardsdatascience.com/reinforcement-learning-w-keras-openai-dqns-1eed3a5338c</t>
+  </si>
+  <si>
+    <t>https://towardsdatascience.com/reinforcement-learning-w-keras-openai-actor-critic-models-f084612cfd69</t>
+  </si>
+  <si>
+    <t>Cleaup DDPG code to align with standard workflow</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Design stardard training/test/visualization workflow for all env/agents</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Cleanup QLearner (discrete/tiles) to align with standard workflow</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Install Linux with OpenAI &amp; Keras for Box2D and Atari Support</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Deep Q Agent with TF for Gym Cartpole</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Deep Q Agent with TF for Gym Acrobat</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Deep Q Agent with TF for Gym Pendulum</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Initial framework for OpenAI training</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DQNv2.0 (Keras instead of TF for simplicity)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Align QQNv2.0 Code with standard workflow</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -114,7 +132,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,13 +166,27 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -184,11 +216,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,200 +506,273 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.125" customWidth="1"/>
+    <col min="1" max="1" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2" s="2">
+        <v>43598</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A2" s="1">
-        <v>43598</v>
-      </c>
-      <c r="B2" s="1">
-        <v>43598</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A4" s="4"/>
+      <c r="B4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A5" s="2">
+        <v>43603</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6" s="2">
+        <v>43604</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D2">
+      <c r="C6" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="2" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A7" s="2">
+        <v>43604</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A8" s="2">
+        <v>43604</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A10" s="5"/>
+      <c r="B10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A11" s="2">
+        <v>43606</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A12" s="2">
+        <v>43606</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A13" s="2">
+        <v>43606</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A14" s="2">
+        <v>43609</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A15" s="2">
+        <v>43609</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A16" s="2">
+        <v>43610</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A5" s="1">
-        <v>43600</v>
-      </c>
-      <c r="B5" s="1">
-        <v>43604</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A6" s="1">
-        <v>43602</v>
-      </c>
-      <c r="B6" s="1">
-        <v>43604</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A7" s="1">
-        <v>43604</v>
-      </c>
-      <c r="B7" s="1">
-        <v>43604</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="C9" s="2" t="s">
+      <c r="C18" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="5">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="5">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="C12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="C13" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A23" s="5"/>
+      <c r="B23" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="C14" t="s">
+      <c r="C23" s="5"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A24" s="5"/>
+      <c r="B24" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="C15" t="s">
+      <c r="C25" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="C16" t="s">
+      <c r="C26" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.4">
-      <c r="C17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.4">
-      <c r="C19" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.4">
-      <c r="C20" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20">
+      <c r="C27" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.4">
-      <c r="C21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.4">
-      <c r="C22" t="s">
-        <v>21</v>
-      </c>
-      <c r="D22">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.4">
-      <c r="D23">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding references to schedule
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F2BDA4-B14A-49BE-A59C-75BABA1F8251}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB942BA-53CD-43C2-A117-2741EABB117C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-13590" yWindow="2325" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Completed</t>
     <phoneticPr fontId="1"/>
@@ -126,13 +126,38 @@
   <si>
     <t>Align QQNv2.0 Code with standard workflow</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>References</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://gym.openai.com/envs/</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://gym.openai.com/envs/Pendulum-v0/</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://github.com/openai/gym/wiki/Leaderboard</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>https://codingvideos.net/using-keras-reinforcement-learning-api-with-openai-gym/</t>
+  </si>
+  <si>
+    <t>https://adventuresinmachinelearning.com/reinforcement-learning-tutorial-python-keras/</t>
+  </si>
+  <si>
+    <t>http://edersantana.github.io/articles/keras_rl/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,6 +199,24 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -213,10 +256,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -226,8 +270,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -506,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -776,9 +823,59 @@
         <v>3</v>
       </c>
     </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B32" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B33" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B34" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B35" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B36" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B38" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B39" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B40" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
+  <hyperlinks>
+    <hyperlink ref="B33" r:id="rId1" xr:uid="{E1DD425F-2C26-4F11-8D3C-B315F2B1CBDC}"/>
+    <hyperlink ref="B34" r:id="rId2" xr:uid="{2518A935-8065-4C76-AEBF-E29BD203F22E}"/>
+    <hyperlink ref="B35" r:id="rId3" xr:uid="{53968899-F652-45A5-A598-2040E812E7E9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>